<commit_message>
Some more results with nested loops
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -101,7 +101,7 @@
     <t>running same as 2 in previous day, but with nested loop and no other changes in the code.</t>
   </si>
   <si>
-    <t>Filtering objects charts were added. Interesting note: all algorithms show great performance due to high filtering of type A. But rereTOUCH shows much better results in filtering another type, but it is not illustrated on performance charts because this improvement is small comparing with filtering of A (or filtering comparing with total filtering of TOUCH). Overall great performance of re*TOUCH algorithms. </t>
+    <t>Filtering objects charts were added. Interesting note: all algorithms show great performance due to high filtering of type A. But rereTOUCH shows much better results in filtering another type, but it is not illustrated on performance charts because this improvement is small comparing with filtering of A (or filtering comparing with total filtering of TOUCH). Overall great performance of re*TOUCH algorithms.</t>
   </si>
   <si>
     <t>reTOUCH and rereTOUCH must be checked separately for best result on different datasets. Comparing with all algorithm does not show their relative improvement.</t>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>Variating fanout (x). Observation variables are the same. Using NL. Objnum = 4000; Epsilon = 5;</t>
+  </si>
+  <si>
+    <t>In total, all algorithms does not have any local minimum variating fanout. TOUCH has some pics. One pick is very significant and calls to the bug 6.12(3)</t>
+  </si>
+  <si>
+    <t>Probably no need to create mathematical equation for best results?</t>
+  </si>
+  <si>
+    <t>Same as previous, but variating leafsize (5-1000-15)</t>
+  </si>
+  <si>
+    <t>If leaf size is not too big (&gt;700-800obj), then timing also remains nearly constant</t>
+  </si>
+  <si>
+    <t>Parameter tuning is actual only in case of Spatial Grid Hash</t>
   </si>
 </sst>
 </file>
@@ -177,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -190,6 +205,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -218,7 +240,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +254,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,10 +338,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:9"/>
+  <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2402,6 +2428,7 @@
       <c r="A3" s="1" t="n">
         <v>24.11</v>
       </c>
+      <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2413,7 +2440,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="4" t="n">
         <v>6.12</v>
       </c>
       <c r="B4" s="1" t="n">
@@ -2430,6 +2457,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
@@ -2444,6 +2472,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="n">
         <v>3</v>
       </c>
@@ -2495,10 +2524,31 @@
       <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
New results (runs on parameter changes)
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -77,7 +77,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -86,7 +85,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> run.</t>
     </r>
@@ -132,6 +130,42 @@
   </si>
   <si>
     <t>Parameter tuning is actual only in case of Spatial Grid Hash</t>
+  </si>
+  <si>
+    <t>Timing and gridSize were fixed, so now running SGH experiments. The same as 6.12 (2,3) (e=5,50), but + SGH building count. Added probing pic, SGH+probing pic, SGH pic</t>
+  </si>
+  <si>
+    <t>dTOUCH and rereTOUCH shows good performance on number of compared objects, but totally they all are the same. Number of A filtered are still the same for all except TOUCH and for B rereTOUCH is the leader. CTOUCH is very heavy on building step. Jet it is not so important, but it does not show so much improvement to consume this time on building step. For some reason dTOUCH consumes less time for building SGH.</t>
+  </si>
+  <si>
+    <t>There was a bug with SGH time adding to join function (in tasks also). Fixed. Building step does not consume so much time. Probing mainly is defined by joinings, that seems very correct now.</t>
+  </si>
+  <si>
+    <t>E = 50 (look previous description)</t>
+  </si>
+  <si>
+    <t>Total time is MUCH bigger. TOUCH again has problems with e=50, objnum=800 (see ..._original pics) : extraordinary slow. All algorithms shows equal performance.</t>
+  </si>
+  <si>
+    <t>resolution of SGH must be consistent with epsilon and typical object size. Otherwise SGH is totally inefficient.</t>
+  </si>
+  <si>
+    <t>Same as (1), but datasets were swapped</t>
+  </si>
+  <si>
+    <t>Number of filtered objects also changes (swapped).</t>
+  </si>
+  <si>
+    <t>Filtering of B less in previous algorithms is the case of datasets, not algorithms themselves.</t>
+  </si>
+  <si>
+    <t>Variating maxLevel coef for dTOUCH. For the reason that in bash I can't work with doubles, I created hard coefficient 1/10 in the code to be able to use smaller delta maxLevel.</t>
+  </si>
+  <si>
+    <t>Constant time for any coefficient. It ssems very strange, so it is either a bug, or nothing is assigned to the second tree nowhere.</t>
+  </si>
+  <si>
+    <t>Probably should run experiment with different epsilon or dataset to catch the difference. Create script for mass producing results if dTOUCH still is interesting.</t>
   </si>
 </sst>
 </file>
@@ -146,7 +180,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -168,14 +201,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -240,7 +271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,6 +289,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,10 +373,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:10"/>
+  <dimension ref="1:14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2545,10 +2580,70 @@
         <v>31</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>8.12</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add paper about random selection
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -85,6 +86,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> run.</t>
     </r>
@@ -166,6 +168,15 @@
   </si>
   <si>
     <t>Probably should run experiment with different epsilon or dataset to catch the difference. Create script for mass producing results if dTOUCH still is interesting.</t>
+  </si>
+  <si>
+    <t>Changing only one dataset (B). Printing script was updated in previous folders, but not here! Copy and modify from 8.12</t>
+  </si>
+  <si>
+    <t>Panos meeting</t>
+  </si>
+  <si>
+    <t>Changing only one dataset (A)</t>
   </si>
 </sst>
 </file>
@@ -180,6 +191,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -201,12 +213,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -373,10 +387,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:14"/>
+  <dimension ref="1:16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="16:16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2460,9 +2474,6 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>24.11</v>
-      </c>
       <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -2522,7 +2533,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="4" t="n">
         <v>7.12</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -2539,6 +2550,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
       <c r="B8" s="1" t="n">
         <v>2</v>
       </c>
@@ -2553,6 +2565,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="n">
         <v>3</v>
       </c>
@@ -2567,6 +2580,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="n">
         <v>4</v>
       </c>
@@ -2639,11 +2653,43 @@
         <v>43</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>9.12</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Many runs and Panos meeting results.
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Dir</t>
   </si>
   <si>
     <t>Experiment description</t>
@@ -178,6 +178,63 @@
   <si>
     <t>Changing only one dataset (A)</t>
   </si>
+  <si>
+    <t>resultsWithDynamicGrid</t>
+  </si>
+  <si>
+    <t>Trying to run first experiment with resolution counting for SGH. Relevant only for cTOUCH, re*TOUCH.</t>
+  </si>
+  <si>
+    <t>Fix SGH and answer Panos question.</t>
+  </si>
+  <si>
+    <t>samples, samplexAxons</t>
+  </si>
+  <si>
+    <t>generated samples from Random distribution and Axons distribution</t>
+  </si>
+  <si>
+    <t>Data used for running experiments</t>
+  </si>
+  <si>
+    <t>The same.</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>running SGH with static resolution + logarithmic scale (semilogy)</t>
+  </si>
+  <si>
+    <t>Inrelevant data</t>
+  </si>
+  <si>
+    <t>Useless job.</t>
+  </si>
+  <si>
+    <t>reresult*</t>
+  </si>
+  <si>
+    <t>Run on Axon and Dendrite dataset. Re and rere touch comparing plots. (4 plot for one picture). Hard-coded generate.py script. Only filtered, MaxNumOfComparisons relevant (SGH is not working correctly)</t>
+  </si>
+  <si>
+    <t>Worst rereTOUCH is better than worst reTOUCH</t>
+  </si>
+  <si>
+    <t>rereTOUCH survives.</t>
+  </si>
+  <si>
+    <t>reresultRandom</t>
+  </si>
+  <si>
+    <t>The same, but with one random distribution. For making possible swapping datasets, using upper-triangular result (for I =1..n, j = I..n).</t>
+  </si>
+  <si>
+    <t>Results are almost equal.</t>
+  </si>
+  <si>
+    <t>Implement rexTOUCH. Limitation for “x” is not very clear yet. Try implemention re3TOUCH first.</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +243,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -221,6 +278,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -285,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,6 +369,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,16 +453,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:16"/>
+  <dimension ref="1:21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="16:16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.02551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8673469387755"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.0102040816326"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="64.8877551020408"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.0102040816326"/>
@@ -2474,6 +2540,7 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
       <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -2595,7 +2662,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="4" t="n">
         <v>8.12</v>
       </c>
       <c r="B11" s="1" t="n">
@@ -2612,6 +2679,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
@@ -2626,6 +2694,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="n">
         <v>3</v>
       </c>
@@ -2640,6 +2709,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="n">
         <v>4</v>
       </c>
@@ -2684,12 +2754,86 @@
         <v>45</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
strange run with dynamic SGH
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -235,6 +235,9 @@
   <si>
     <t>Implement rexTOUCH. Limitation for “x” is not very clear yet. Try implemention re3TOUCH first.</t>
   </si>
+  <si>
+    <t>Using runTest from previous experiment. Generated random datasets are copied to ./data/ folder, where can be used by next runs. RunTestRandom executes tests on generated test on Uniformly Random dataset (one file). Because of using one file, -ge (great or equal) flag is used (do not swap two datasamples) (look 16.12 reresultRandom).</t>
+  </si>
 </sst>
 </file>
 
@@ -243,7 +246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -278,11 +281,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -347,7 +345,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,10 +367,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,17 +447,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:21"/>
+  <dimension ref="1:22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.02551020408163"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.0102040816326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="64.8877551020408"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.0102040816326"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="2" width="35.0102040816326"/>
@@ -1505,7 +1499,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>23.11</v>
       </c>
@@ -2539,7 +2533,7 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
@@ -2552,7 +2546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>6.12</v>
       </c>
@@ -2631,7 +2625,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="n">
         <v>3</v>
@@ -2723,8 +2717,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
         <v>9.12</v>
       </c>
       <c r="B15" s="1" t="n">
@@ -2741,6 +2735,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="n">
         <v>2</v>
       </c>
@@ -2754,11 +2749,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16.12</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2799,7 +2794,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
@@ -2813,7 +2808,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
         <v>62</v>
       </c>
@@ -2825,6 +2820,14 @@
       </c>
       <c r="E21" s="1" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>22.12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more strange results. UD/BU traversal. reTOUCH dyn grid experiment.
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -244,6 +244,33 @@
   <si>
     <t>Very strange results. Seems as a lot of bugs.</t>
   </si>
+  <si>
+    <t>Axons</t>
+  </si>
+  <si>
+    <t>The same as previous random, but with axons and dendrites. Program was updated. Zero localPartitioning means using dynamic grid. </t>
+  </si>
+  <si>
+    <t>Better results. Due to time constraints, only up to 6000 size subsets was considered. Some problems with dTOUCH assignment</t>
+  </si>
+  <si>
+    <t>TraversalType</t>
+  </si>
+  <si>
+    <t>Manually renaming in this experiments and results second half of results as “reTOUCH &lt;type of traversal&gt;”. This compares BU (bottom-up) and UD (up-down) traversals of the tree for reTOUCH and for dynamic grid.</t>
+  </si>
+  <si>
+    <t>Number of sonsidered objects for dataset 6000 is different, so resuts for 6000 can be inaccurate. Overall, results are strange. BU shows better results, however number of compared results for UD is much smaller.</t>
+  </si>
+  <si>
+    <t>dynamicForReTouch</t>
+  </si>
+  <si>
+    <t>check dynamic performance for reTOUCH for UD traversal. Manually rename second half of results.</t>
+  </si>
+  <si>
+    <t>E1 shown decreasing of compared objects. All show increasing total time. Dynamic SGH shows bad performance.</t>
+  </si>
 </sst>
 </file>
 
@@ -252,7 +279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -287,6 +314,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -351,7 +383,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,6 +405,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,10 +489,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:22"/>
+  <dimension ref="1:25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2846,13 +2882,50 @@
         <v>68</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>24.12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Join traversal type camparison runs
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -248,7 +248,7 @@
     <t>Axons</t>
   </si>
   <si>
-    <t>The same as previous random, but with axons and dendrites. Program was updated. Zero localPartitioning means using dynamic grid. </t>
+    <t>The same as previous random, but with axons and dendrites. Program was updated. Zero localPartitioning means using dynamic grid.</t>
   </si>
   <si>
     <t>Better results. Due to time constraints, only up to 6000 size subsets was considered. Some problems with dTOUCH assignment</t>
@@ -270,6 +270,42 @@
   </si>
   <si>
     <t>E1 shown decreasing of compared objects. All show increasing total time. Dynamic SGH shows bad performance.</t>
+  </si>
+  <si>
+    <t>fanout</t>
+  </si>
+  <si>
+    <t>Dynamic grid, Axon/Dendrite samples, Top-Down traversal. Fanout is a parameter. 5 algorithms considered. TOUCH is very bad, so plotting without it. Plots only for one object size and epsilon, however results obtained for many values of both of them. </t>
+  </si>
+  <si>
+    <t>No any dependence observed.</t>
+  </si>
+  <si>
+    <t>leafsize</t>
+  </si>
+  <si>
+    <t>traveralTypeRandomSizeConstantGrid</t>
+  </si>
+  <si>
+    <t>SampleGenerator modified, ONLY Box has new feature – random expand of size of objects (larger deviation). New Samples generated from uniform distribution. Using this set of samples new experiment with dynamic grid was run (other same as traversal).</t>
+  </si>
+  <si>
+    <t>traversalType</t>
+  </si>
+  <si>
+    <t>3 cases of tree traversal with reTOUCH algorithm is implemented. One more case is imported from traversalTypeCase3WithFiltering. Now 4 cases: case 1, case 3, case 4, case 3 with filtering (using filtering as Box::overlap(childEntry-&gt;mbr, targetNode-&gt;mbr)). Many epsilon are considered, plotting only one epsilon. DynamicGrid using. </t>
+  </si>
+  <si>
+    <t>traversalTypeCase3WithFiltering</t>
+  </si>
+  <si>
+    <t>see traversalType</t>
+  </si>
+  <si>
+    <t>traversalTypeWithConstantGrid</t>
+  </si>
+  <si>
+    <t>Same as traversalType, but with constantGrid.</t>
   </si>
 </sst>
 </file>
@@ -279,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -314,11 +350,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -383,7 +414,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -405,10 +436,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,10 +516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:25"/>
+  <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2900,7 +2927,7 @@
       <c r="B24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -2918,14 +2945,72 @@
         <v>77</v>
       </c>
     </row>
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>28.12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
more experiments with all algorithms
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -315,6 +315,24 @@
   </si>
   <si>
     <t>A bug in the code was found and all results was rerun (using only one epsilon value)</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>additional algorithms added.</t>
+  </si>
+  <si>
+    <t>Problems with Sgrid (too fast) and TOUCH (also too fast)</t>
+  </si>
+  <si>
+    <t>..Dynamic</t>
+  </si>
+  <si>
+    <t>New Sgrid for local dynamic is presented</t>
+  </si>
+  <si>
+    <t>Problems with TOUCH – too slow</t>
   </si>
 </sst>
 </file>
@@ -525,10 +543,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:32"/>
+  <dimension ref="1:34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3024,8 +3042,33 @@
         <v>92</v>
       </c>
     </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>8.01</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
@@ -3033,6 +3076,7 @@
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
looking for type best type traversal. experiments.
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -338,10 +338,34 @@
     <t>…</t>
   </si>
   <si>
-    <t>Name of the folder show the parameters. </t>
-  </si>
-  <si>
-    <t>TOUCH is the best on big algorithms – one problem less. New problem: no any *TOUCH algorithms except reTOUCH (maybe rereTOUCH, I didn't checked) survive on big dataset with error of “out of memory”. </t>
+    <t>Name of the folder show the parameters.</t>
+  </si>
+  <si>
+    <t>TOUCH is the best on big algorithms – one problem less. New problem: no any *TOUCH algorithms except reTOUCH (maybe rereTOUCH, I didn't checked) survive on big dataset with error of “out of memory”.</t>
+  </si>
+  <si>
+    <t>Different experiments with grid sizes. For debugging and for showing basics advantage of D2 in front of D1.</t>
+  </si>
+  <si>
+    <t>D2 is better.</t>
+  </si>
+  <si>
+    <t>D3 is needed.</t>
+  </si>
+  <si>
+    <t>CheckAllTraversal...</t>
+  </si>
+  <si>
+    <t>Different types of dynamic grid with Axon/Dendrite data samples and e = 10</t>
+  </si>
+  <si>
+    <t>No significant difference between D2 and D3</t>
+  </si>
+  <si>
+    <t>SGType</t>
+  </si>
+  <si>
+    <t>Random expanded data samples and epsilon = 50</t>
   </si>
 </sst>
 </file>
@@ -556,10 +580,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:35"/>
+  <dimension ref="1:38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3066,7 +3090,7 @@
       <c r="D32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="4" t="n">
         <v>8.01</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -3080,6 +3104,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
         <v>96</v>
       </c>
@@ -3102,6 +3127,45 @@
       </c>
       <c r="D35" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>12.01</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>16.01</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experiments for final runs. looking for best performance of our algorithms.
</commit_message>
<xml_diff>
--- a/run/Journal.xlsx
+++ b/run/Journal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>Random expanded data samples and epsilon = 50</t>
+  </si>
+  <si>
+    <t>...Small</t>
+  </si>
+  <si>
+    <t>Random expanding is taking place now for each of dimension separately</t>
   </si>
 </sst>
 </file>
@@ -580,10 +586,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:38"/>
+  <dimension ref="1:40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2972,6 +2978,7 @@
       <c r="D22" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="E22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
@@ -2986,6 +2993,7 @@
       <c r="D23" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="E23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
@@ -2998,6 +3006,7 @@
       <c r="D24" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="E24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
@@ -3010,6 +3019,7 @@
       <c r="D25" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="E25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
@@ -3024,6 +3034,7 @@
       <c r="D26" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="E26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
@@ -3036,6 +3047,7 @@
       <c r="D27" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="E27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
@@ -3048,6 +3060,7 @@
       <c r="D28" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="E28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
@@ -3058,6 +3071,7 @@
         <v>86</v>
       </c>
       <c r="D29" s="6"/>
+      <c r="E29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
@@ -3068,6 +3082,7 @@
         <v>88</v>
       </c>
       <c r="D30" s="6"/>
+      <c r="E30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
@@ -3078,6 +3093,7 @@
         <v>90</v>
       </c>
       <c r="D31" s="6"/>
+      <c r="E31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
@@ -3088,6 +3104,7 @@
         <v>92</v>
       </c>
       <c r="D32" s="6"/>
+      <c r="E32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
@@ -3102,6 +3119,7 @@
       <c r="D33" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="E33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
@@ -3114,6 +3132,7 @@
       <c r="D34" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="E34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -3128,6 +3147,7 @@
       <c r="D35" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="E35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -3168,8 +3188,24 @@
         <v>109</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>17.01</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
@@ -3178,6 +3214,7 @@
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A37:A39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>